<commit_message>
lab1 + hw lesson2 + scripts start
</commit_message>
<xml_diff>
--- a/lesson2/lesson2.xlsx
+++ b/lesson2/lesson2.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="16">
   <si>
     <t>случайная выборка</t>
   </si>
@@ -139,13 +139,13 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -385,11 +385,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="5938448"/>
-        <c:axId val="5928656"/>
+        <c:axId val="-40247488"/>
+        <c:axId val="-40253472"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="5938448"/>
+        <c:axId val="-40247488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -446,12 +446,12 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="5928656"/>
+        <c:crossAx val="-40253472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="5928656"/>
+        <c:axId val="-40253472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -508,7 +508,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="5938448"/>
+        <c:crossAx val="-40247488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1413,25 +1413,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="F89" sqref="F89"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="H85" sqref="H85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="33.42578125" customWidth="1"/>
+    <col min="7" max="7" width="19.5703125" customWidth="1"/>
+    <col min="8" max="8" width="24.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
@@ -1527,272 +1529,356 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2</v>
       </c>
       <c r="B32">
         <v>2</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="D32" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E32" s="4"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E32" s="3"/>
+      <c r="G32" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H32" s="3"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>1</v>
       </c>
       <c r="B33">
         <v>1</v>
       </c>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>3</v>
       </c>
       <c r="B34">
         <v>3</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="D34" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E34" s="2">
+      <c r="E34" s="1">
         <v>1.96</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G34" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H34" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>12</v>
       </c>
       <c r="B35">
         <v>1</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="D35" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E35" s="2">
+      <c r="E35" s="1">
         <v>0.25482019804821854</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G35" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H35" s="1">
+        <v>0.2581988897471611</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>1</v>
       </c>
       <c r="B36">
         <v>2</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="D36" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E36" s="2">
+      <c r="E36" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G36" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H36" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>24</v>
       </c>
       <c r="B37">
         <v>1</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="D37" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E37" s="2">
+      <c r="E37" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G37" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H37" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>3</v>
       </c>
       <c r="B38">
         <v>2</v>
       </c>
-      <c r="D38" s="2" t="s">
+      <c r="D38" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E38" s="2">
+      <c r="E38" s="1">
         <v>1.2741009902410927</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G38" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H38" s="1">
+        <v>1.2909944487358056</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>5</v>
       </c>
       <c r="B39">
         <v>4</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="D39" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E39" s="2">
+      <c r="E39" s="1">
         <v>1.6233333333333331</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G39" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H39" s="1">
+        <v>1.6666666666666667</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>3</v>
       </c>
       <c r="B40">
         <v>3</v>
       </c>
-      <c r="D40" s="2" t="s">
+      <c r="D40" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E40" s="2">
+      <c r="E40" s="1">
         <v>0.12104742041402483</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G40" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H40" s="1">
+        <v>-0.10079051383399129</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B41">
         <v>5</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="D41" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E41" s="2">
+      <c r="E41" s="1">
         <v>0.4746620841766197</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G41" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H41" s="1">
+        <v>0.37887880560724729</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B42">
         <v>3</v>
       </c>
-      <c r="D42" s="2" t="s">
+      <c r="D42" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E42" s="2">
+      <c r="E42" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G42" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H42" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B43">
         <v>2</v>
       </c>
-      <c r="D43" s="2" t="s">
+      <c r="D43" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E43" s="2">
+      <c r="E43" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G43" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H43" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B44">
         <v>2</v>
       </c>
-      <c r="D44" s="2" t="s">
+      <c r="D44" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E44" s="2">
+      <c r="E44" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G44" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H44" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B45">
         <v>2</v>
       </c>
-      <c r="D45" s="2" t="s">
+      <c r="D45" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E45" s="2">
+      <c r="E45" s="1">
         <v>49</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G45" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H45" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B46">
         <v>1</v>
       </c>
-      <c r="D46" s="2" t="s">
+      <c r="D46" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E46" s="2">
+      <c r="E46" s="1">
         <v>25</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G46" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H46" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B47">
         <v>2</v>
       </c>
-      <c r="D47" s="3" t="s">
+      <c r="D47" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E47" s="3">
+      <c r="E47" s="2">
         <v>0.52592304022548686</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B48">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.25">

</xml_diff>